<commit_message>
The code for project is updated
</commit_message>
<xml_diff>
--- a/SendingMailFromExcell/STUDENTS& COURSE DETAILS FOR CRACKJOB.xlsx
+++ b/SendingMailFromExcell/STUDENTS& COURSE DETAILS FOR CRACKJOB.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{69791EA4-D11B-492B-8D5E-999B1BB71100}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="6480" windowWidth="9585" xWindow="0" yWindow="2520"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="9670" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="STUDENT_DETAILS" r:id="rId1" sheetId="1"/>
-    <sheet name="COURSE_DETAILS" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="STUDENT_DETAILS" sheetId="1" r:id="rId1"/>
+    <sheet name="COURSE_DETAILS" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <oleSize ref="A1:M20"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="86">
   <si>
     <t>STUDENT_ID</t>
   </si>
@@ -236,9 +237,6 @@
   </si>
   <si>
     <t>BasakA@8.436148129E9</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>yes</t>
@@ -283,9 +281,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,23 +316,31 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -344,10 +349,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -382,7 +387,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,9 +419,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -448,6 +471,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -503,7 +544,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -512,13 +553,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -528,7 +569,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -537,7 +578,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -546,7 +587,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -556,12 +597,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -592,7 +633,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -611,7 +652,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -623,23 +664,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="25.9921875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="17.03515625" collapsed="true"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,9 +724,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -721,15 +762,15 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>83</v>
-      </c>
-      <c r="N2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>84</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -765,13 +806,13 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -812,10 +853,10 @@
         <v>61</v>
       </c>
       <c r="N4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -853,13 +894,13 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -900,10 +941,10 @@
         <v>63</v>
       </c>
       <c r="N6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -944,10 +985,10 @@
         <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -988,39 +1029,39 @@
         <v>72</v>
       </c>
       <c r="N8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>67</v>
       </c>
       <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
       </c>
       <c r="D9" s="1">
         <v>40154</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9">
         <v>7205186494</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H9">
         <v>2010</v>
       </c>
       <c r="I9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K9" t="s">
         <v>36</v>
@@ -1029,38 +1070,38 @@
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
-    <hyperlink r:id="rId2" ref="E8"/>
-    <hyperlink r:id="rId3" ref="M8"/>
-    <hyperlink r:id="rId4" ref="E9"/>
-    <hyperlink r:id="rId5" ref="E3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1083,7 +1124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1129,7 +1170,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1152,7 +1193,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1175,7 +1216,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1199,18 +1240,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>